<commit_message>
V402 Photozelle tabellen im anhang
</commit_message>
<xml_diff>
--- a/V402/Daten/photozelle_kennlinie.xlsx
+++ b/V402/Daten/photozelle_kennlinie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="365_1"/>
@@ -57,7 +57,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -89,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -99,12 +99,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="2" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,7 +431,7 @@
       <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>0.5</v>
       </c>
     </row>
@@ -627,7 +621,7 @@
     <col min="3" max="3" style="3" width="9.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2">
         <v>78</v>
       </c>
@@ -649,7 +643,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2">
         <v>65</v>
       </c>
@@ -660,7 +654,7 @@
         <v>33.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2">
         <v>44</v>
       </c>
@@ -671,7 +665,7 @@
         <v>68.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2">
         <v>30</v>
       </c>
@@ -682,7 +676,7 @@
         <v>104.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2">
         <v>12</v>
       </c>
@@ -693,7 +687,7 @@
         <v>156.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -704,7 +698,7 @@
         <v>202.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2">
         <v>-9</v>
       </c>
@@ -715,7 +709,7 @@
         <v>257.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2">
         <v>-17</v>
       </c>
@@ -726,7 +720,7 @@
         <v>318.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2">
         <v>-22.2</v>
       </c>
@@ -737,7 +731,7 @@
         <v>434</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2">
         <v>-23.4</v>
       </c>
@@ -748,7 +742,7 @@
         <v>676</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2">
         <v>-23.4</v>
       </c>
@@ -1417,7 +1411,7 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1574,7 +1568,7 @@
         <v>-21.1</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C14" s="2">
         <v>2782</v>
@@ -1815,12 +1809,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2625,7 +2619,7 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>